<commit_message>
upload mapa y fake
</commit_message>
<xml_diff>
--- a/docs/reportes_minsa.xlsx
+++ b/docs/reportes_minsa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseincio/Documents/Sites/Git_repo/COVID_19_PERU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D652C8-7FC2-D44B-96A1-98B21BF85415}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780F1732-CA73-F947-B98B-85B56FC0F61B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27520" yWindow="460" windowWidth="25440" windowHeight="14380" xr2:uid="{0852571F-0CF6-4B4E-96BA-A023FDA95ADA}"/>
+    <workbookView xWindow="27520" yWindow="460" windowWidth="25440" windowHeight="14380" activeTab="1" xr2:uid="{0852571F-0CF6-4B4E-96BA-A023FDA95ADA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="20">
   <si>
     <t>Dia</t>
   </si>
@@ -58,6 +58,42 @@
   </si>
   <si>
     <t>Recuperados</t>
+  </si>
+  <si>
+    <t>Departamento</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>LIMA</t>
+  </si>
+  <si>
+    <t>CALLAO</t>
+  </si>
+  <si>
+    <t>ANCASH</t>
+  </si>
+  <si>
+    <t>AREQUIPA</t>
+  </si>
+  <si>
+    <t>CUSCO</t>
+  </si>
+  <si>
+    <t>HUANUCO</t>
+  </si>
+  <si>
+    <t>ICA</t>
+  </si>
+  <si>
+    <t>LA LIBERTAD</t>
+  </si>
+  <si>
+    <t>LAMBAYEQUE</t>
+  </si>
+  <si>
+    <t>PIURA</t>
   </si>
 </sst>
 </file>
@@ -424,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7AA3A2-91DD-F943-ABC3-A3878B7085E5}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -839,14 +875,436 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE914600-E178-F246-8CE3-28010C754450}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>58</v>
+      </c>
+      <c r="C2" s="1">
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>70</v>
+      </c>
+      <c r="C12" s="1">
+        <v>43906</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>43906</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>43906</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>43906</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1">
+        <v>43906</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1">
+        <v>43906</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>43906</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1">
+        <v>43906</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>43906</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1">
+        <v>43906</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <v>37</v>
+      </c>
+      <c r="C22" s="1">
+        <v>43904</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1">
+        <v>43904</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1">
+        <v>43904</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1">
+        <v>43904</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
+        <v>43904</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27">
+        <v>32</v>
+      </c>
+      <c r="C27" s="1">
+        <v>43903</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" s="1">
+        <v>43903</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1">
+        <v>43903</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30" s="1">
+        <v>43903</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1">
+        <v>43903</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32">
+        <v>22</v>
+      </c>
+      <c r="C32" s="1">
+        <v>43902</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33">
+        <v>17</v>
+      </c>
+      <c r="C33" s="1">
+        <v>43901</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34">
+        <v>11</v>
+      </c>
+      <c r="C34" s="1">
+        <v>43900</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35">
+        <v>9</v>
+      </c>
+      <c r="C35" s="1">
+        <v>43899</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36">
+        <v>7</v>
+      </c>
+      <c r="C36" s="1">
+        <v>43898</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" s="1">
+        <v>43897</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38">
+        <v>6</v>
+      </c>
+      <c r="C38" s="1">
+        <v>43896</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>